<commit_message>
Fiscal Performance Information cleaned
</commit_message>
<xml_diff>
--- a/Datasets/List_of_Possible_Data_Sets.xlsx
+++ b/Datasets/List_of_Possible_Data_Sets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dda39ef004021ca5/Documents/GitHub/Hertie_School_MDS_Master_Thesis/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="216" documentId="8_{3161AA99-2E20-4B85-8449-7A266E90B51F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AACB2CA-A4C2-4F28-AAC3-AC9CC89D3263}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{0F659CC4-FC61-4FCB-A4E7-CFAA2C0E1B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-5520" windowWidth="29040" windowHeight="17520" xr2:uid="{1E935717-DD72-45D7-9C68-C9ACEFDD9922}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{1E935717-DD72-45D7-9C68-C9ACEFDD9922}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1132,7 +1132,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>